<commit_message>
Practica 05: HOLA LCD Completa :fire:
</commit_message>
<xml_diff>
--- a/TIMER Notas Musicales.xlsx
+++ b/TIMER Notas Musicales.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaimo\Documents\ESCOM\7o Semestre\04 Microcontroladores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaimo\Documents\Github\Microcontrollers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3831968A-40D0-4AA2-9709-839A784C4BE2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073564D6-1FDB-416A-8CE6-E2A77501324E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{A94A70E5-2627-457F-9DE1-AA5DE15F0522}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Preescala</t>
   </si>
@@ -186,6 +186,9 @@
       </rPr>
       <t>preescalador</t>
     </r>
+  </si>
+  <si>
+    <t>Estos valores van en el ensamblador</t>
   </si>
 </sst>
 </file>
@@ -317,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -327,13 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -355,26 +352,107 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -412,18 +490,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A7F2932D-D6EE-4E96-8001-5BB00FFBC4AE}" name="Tabla4" displayName="Tabla4" ref="A12:I16" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A7F2932D-D6EE-4E96-8001-5BB00FFBC4AE}" name="Tabla4" displayName="Tabla4" ref="A12:I17" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A12:I16" xr:uid="{0FD17AD3-83D1-425E-BCC6-FC61EAF13920}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{63D2065A-C412-43E1-9BE4-EBD9663080EC}" name="Preescala" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{1AF59A16-F1CF-4BDC-83E3-19956FCC1A1B}" name="Fpreescalador" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{28E3B38C-DB7A-4BE8-8AA5-071C3C92CC5C}" name="PRx (DO)" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{637415A1-859B-4F35-A1ED-5C21F78AF99E}" name="PRx (RE)" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{CCF8132E-A5D5-4DA5-843A-B004408AFEAD}" name="PRx (MI)" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{56000FD9-F2E3-414D-9B47-E58C4D4AC25D}" name="PRx (FA)" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{9A0E24CC-6AC9-4FCD-A80A-67D49C8B9E99}" name="PRx (SOL)" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{BBBEB1C5-EE08-4780-9A2F-80E50C30A011}" name="PRx (LA)" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{6D4ADE8D-368B-47A2-B1A5-6BE442B86104}" name="PRx (SI)" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{63D2065A-C412-43E1-9BE4-EBD9663080EC}" name="Preescala" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{1AF59A16-F1CF-4BDC-83E3-19956FCC1A1B}" name="Fpreescalador" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{28E3B38C-DB7A-4BE8-8AA5-071C3C92CC5C}" name="PRx (DO)" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
+      <totalsRowFormula xml:space="preserve"> ROUND(C15,0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{637415A1-859B-4F35-A1ED-5C21F78AF99E}" name="PRx (RE)" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+      <totalsRowFormula>ROUND(D15,0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{CCF8132E-A5D5-4DA5-843A-B004408AFEAD}" name="PRx (MI)" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+      <totalsRowFormula>ROUND(E16,0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{56000FD9-F2E3-414D-9B47-E58C4D4AC25D}" name="PRx (FA)" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+      <totalsRowFormula>ROUND(F13,0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{9A0E24CC-6AC9-4FCD-A80A-67D49C8B9E99}" name="PRx (SOL)" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+      <totalsRowFormula>ROUND(G13,0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{BBBEB1C5-EE08-4780-9A2F-80E50C30A011}" name="PRx (LA)" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+      <totalsRowFormula>ROUND(H14,0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{6D4ADE8D-368B-47A2-B1A5-6BE442B86104}" name="PRx (SI)" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+      <totalsRowFormula>ROUND(I13,0)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -729,7 +821,7 @@
   <dimension ref="A2:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,23 +844,23 @@
       <c r="B2">
         <v>1843200</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="J2" s="14" t="s">
+      <c r="H2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -782,172 +874,172 @@
       <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="15">
         <v>261.62556499999999</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="7">
+      <c r="F3" s="15"/>
+      <c r="G3" s="16">
         <f xml:space="preserve"> 2 * E3</f>
         <v>523.25112999999999</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="16"/>
       <c r="I3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="5"/>
       <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="15">
         <v>293.66476799999998</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="7">
+      <c r="F4" s="15"/>
+      <c r="G4" s="16">
         <f t="shared" ref="G4:G9" si="0" xml:space="preserve"> 2 * E4</f>
         <v>587.32953599999996</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="5"/>
       <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="15">
         <v>329.62755700000002</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="7">
+      <c r="F5" s="15"/>
+      <c r="G5" s="16">
         <f t="shared" si="0"/>
         <v>659.25511400000005</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15" t="s">
+      <c r="H5" s="16"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="5"/>
       <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="15">
         <v>349.22823099999999</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="7">
+      <c r="F6" s="15"/>
+      <c r="G6" s="16">
         <f t="shared" si="0"/>
         <v>698.45646199999999</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="5"/>
       <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="15">
         <v>391.99543599999998</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="7">
+      <c r="F7" s="15"/>
+      <c r="G7" s="16">
         <f t="shared" si="0"/>
         <v>783.99087199999997</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15" t="s">
+      <c r="H7" s="16"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="5"/>
       <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="16">
         <v>440</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7">
+      <c r="F8" s="16"/>
+      <c r="G8" s="16">
         <f t="shared" si="0"/>
         <v>880</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="5"/>
       <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="15">
         <v>493.88310100000001</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="7">
+      <c r="F9" s="15"/>
+      <c r="G9" s="16">
         <f t="shared" si="0"/>
         <v>987.76620200000002</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
       <c r="N9" s="3"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -986,7 +1078,7 @@
         <f xml:space="preserve"> B2/A13</f>
         <v>1843200</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="6">
         <f xml:space="preserve"> B13/G3</f>
         <v>3522.5915326738045</v>
       </c>
@@ -1126,258 +1218,294 @@
         <v>7.2891742857992625</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="12">
+        <f xml:space="preserve"> ROUND(C15,0)</f>
+        <v>55</v>
+      </c>
+      <c r="D17" s="12">
+        <f>ROUND(D15,0)</f>
+        <v>49</v>
+      </c>
+      <c r="E17" s="12">
+        <f>ROUND(E16,0)</f>
+        <v>11</v>
+      </c>
+      <c r="F17" s="12">
+        <f>ROUND(F13,0)</f>
+        <v>2639</v>
+      </c>
+      <c r="G17" s="12">
+        <f>ROUND(G13,0)</f>
+        <v>2351</v>
+      </c>
+      <c r="H17" s="12">
+        <f>ROUND(H14,0)</f>
+        <v>262</v>
+      </c>
+      <c r="I17" s="12">
+        <f>ROUND(I13,0)</f>
+        <v>1866</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
         <v>1</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="8">
         <f>B2/A19</f>
         <v>1843200</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="13">
         <f>ROUND(C13,0)</f>
         <v>3523</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="13">
         <f t="shared" ref="D19:I19" si="1">ROUND(D13,0)</f>
         <v>3138</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="13">
         <f t="shared" si="1"/>
         <v>2796</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="13">
         <f t="shared" si="1"/>
         <v>2639</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="13">
         <f t="shared" si="1"/>
         <v>2351</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="13">
         <f t="shared" si="1"/>
         <v>2095</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="13">
         <f t="shared" si="1"/>
         <v>1866</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
         <v>8</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="8">
         <f>B2/A20</f>
         <v>230400</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="13">
         <f t="shared" ref="C20:I22" si="2">ROUND(C14,0)</f>
         <v>440</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <f t="shared" si="2"/>
         <v>392</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="13">
         <f t="shared" si="2"/>
         <v>349</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="13">
         <f t="shared" si="2"/>
         <v>330</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="13">
         <f t="shared" si="2"/>
         <v>294</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="13">
         <f t="shared" si="2"/>
         <v>262</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="13">
         <f t="shared" si="2"/>
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
         <v>64</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="8">
         <f>B2/A21</f>
         <v>28800</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="13">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="13">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="13">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="13">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G21" s="13">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="13">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I21" s="13">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
         <v>256</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="8">
         <f>B2/A22</f>
         <v>7200</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="13">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="13">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="13">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="13">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G22" s="13">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="13">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="13">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="9" t="s">
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="I24" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="10">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="8">
         <v>1</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="13">
         <f>ABS(C19-C13)</f>
         <v>0.40846732619547765</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="13">
         <f t="shared" ref="D25:I25" si="3">ABS(D19-D13)</f>
         <v>0.27227650270970116</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="13">
         <f t="shared" si="3"/>
         <v>0.11725164106974262</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="14">
         <f t="shared" si="3"/>
         <v>3.8088584539309522E-2</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="14">
         <f t="shared" si="3"/>
         <v>4.7781076716546522E-2</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="13">
         <f t="shared" si="3"/>
         <v>0.45454545454549589</v>
       </c>
-      <c r="I25" s="17">
+      <c r="I25" s="14">
         <f t="shared" si="3"/>
         <v>2.8617164611205226E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="11">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="9">
         <v>8</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="13">
         <f>ABS(C20-C14)</f>
         <v>0.32394158422556529</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="13">
         <f t="shared" ref="D26:I26" si="4">ABS(D20-D14)</f>
         <v>0.28403456283871265</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="13">
         <f t="shared" si="4"/>
         <v>0.48534354486628217</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="13">
         <f t="shared" si="4"/>
         <v>0.12976107306741369</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="13">
         <f t="shared" si="4"/>
         <v>0.11902736541043168</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H26" s="14">
         <f t="shared" si="4"/>
         <v>0.18181818181818699</v>
       </c>
-      <c r="I26" s="16">
+      <c r="I26" s="13">
         <f t="shared" si="4"/>
         <v>0.25357714557640065</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="10">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="8">
         <v>64</v>
       </c>
       <c r="C27" s="1">
@@ -1409,8 +1537,8 @@
         <v>0.15669714319705008</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12">
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10">
         <v>256</v>
       </c>
       <c r="C28">
@@ -1442,41 +1570,41 @@
         <v>0.28917428579926252</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="13">
         <f>MIN(C25:C28)</f>
         <v>4.0492698028195662E-2</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="13">
         <f>MIN(D25:D28)</f>
         <v>3.5504320354839081E-2</v>
       </c>
-      <c r="E30" s="16">
-        <f t="shared" ref="D30:I30" si="7">MIN(E25:E28)</f>
+      <c r="E30" s="13">
+        <f t="shared" ref="E30:I30" si="7">MIN(E25:E28)</f>
         <v>7.8583014222928682E-2</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="13">
         <f t="shared" si="7"/>
         <v>3.8088584539309522E-2</v>
       </c>
-      <c r="G30" s="16">
+      <c r="G30" s="13">
         <f t="shared" si="7"/>
         <v>4.7781076716546522E-2</v>
       </c>
-      <c r="H30" s="16">
+      <c r="H30" s="13">
         <f t="shared" si="7"/>
         <v>0.18181818181818166</v>
       </c>
-      <c r="I30" s="16">
+      <c r="I30" s="13">
         <f t="shared" si="7"/>
         <v>2.8617164611205226E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="9" t="s">
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="3">
@@ -1502,7 +1630,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="I7:I9"/>
     <mergeCell ref="J2:M2"/>
@@ -1510,11 +1640,7 @@
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="J5:M6"/>
     <mergeCell ref="J7:M9"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="J17:L17"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="C11:I11"/>
@@ -1527,6 +1653,9 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>